<commit_message>
Base admin panel (frontend), carpeta page renombrada, modulo layout
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DC8832-7CAB-447F-89EB-544AD16339E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66741E8D-68B0-44AD-BBF8-9B4D8439138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1086,6 +1086,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1118,21 +1133,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:Z1037"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1685,17 +1685,17 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="94"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="99"/>
       <c r="J11" s="3"/>
       <c r="K11" s="12"/>
       <c r="L11" s="3"/>
@@ -1715,31 +1715,31 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="104" t="s">
+      <c r="E12" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="87">
         <v>44559</v>
       </c>
-      <c r="G12" s="105">
+      <c r="G12" s="87">
         <v>44560</v>
       </c>
-      <c r="H12" s="103">
+      <c r="H12" s="85">
         <v>1</v>
       </c>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="86" t="s">
         <v>129</v>
       </c>
       <c r="J12" s="13" t="s">
@@ -1763,31 +1763,31 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="105">
+      <c r="F13" s="87">
         <v>44559</v>
       </c>
-      <c r="G13" s="105">
+      <c r="G13" s="87">
         <v>44560</v>
       </c>
-      <c r="H13" s="103">
+      <c r="H13" s="85">
         <v>1</v>
       </c>
-      <c r="I13" s="104" t="s">
+      <c r="I13" s="86" t="s">
         <v>129</v>
       </c>
       <c r="J13" s="13" t="s">
@@ -1811,31 +1811,31 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="104" t="s">
+      <c r="E14" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="105">
+      <c r="F14" s="87">
         <v>44559</v>
       </c>
-      <c r="G14" s="105">
+      <c r="G14" s="87">
         <v>44560</v>
       </c>
-      <c r="H14" s="103">
+      <c r="H14" s="85">
         <v>1</v>
       </c>
-      <c r="I14" s="104" t="s">
+      <c r="I14" s="86" t="s">
         <v>129</v>
       </c>
       <c r="J14" s="13" t="s">
@@ -1859,31 +1859,31 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="104" t="s">
+      <c r="E15" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="105">
+      <c r="F15" s="87">
         <v>44559</v>
       </c>
-      <c r="G15" s="105">
+      <c r="G15" s="87">
         <v>44560</v>
       </c>
-      <c r="H15" s="103">
+      <c r="H15" s="85">
         <v>1</v>
       </c>
-      <c r="I15" s="104" t="s">
+      <c r="I15" s="86" t="s">
         <v>129</v>
       </c>
       <c r="J15" s="13" t="s">
@@ -1932,7 +1932,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="68" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1978,7 +1978,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="68" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2024,7 +2024,7 @@
         <v>4</v>
       </c>
       <c r="I18" s="68" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2070,7 +2070,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="68" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2116,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="68" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2162,7 +2162,7 @@
         <v>4</v>
       </c>
       <c r="I21" s="73" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2208,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="73" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2254,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="73" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2300,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="I24" s="73" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2346,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="73" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2392,7 +2392,7 @@
         <v>4</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2438,7 +2438,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2622,7 +2622,7 @@
         <v>4</v>
       </c>
       <c r="I31" s="58" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2668,7 +2668,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="58" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -4091,12 +4091,12 @@
       <c r="Z64" s="3"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="84" t="s">
+      <c r="A65" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B65" s="85"/>
-      <c r="C65" s="85"/>
-      <c r="D65" s="86"/>
+      <c r="B65" s="90"/>
+      <c r="C65" s="90"/>
+      <c r="D65" s="91"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -4121,10 +4121,10 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="95" t="s">
+      <c r="A66" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="B66" s="86"/>
+      <c r="B66" s="91"/>
       <c r="C66" s="51" t="s">
         <v>89</v>
       </c>
@@ -4155,17 +4155,17 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="97"/>
+      <c r="B67" s="102"/>
       <c r="C67" s="55" t="s">
         <v>127</v>
       </c>
       <c r="D67" s="27">
         <v>2</v>
       </c>
-      <c r="E67" s="106" t="s">
+      <c r="E67" s="88" t="s">
         <v>136</v>
       </c>
       <c r="F67" s="3"/>
@@ -4191,17 +4191,17 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="96" t="s">
+      <c r="A68" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="B68" s="97"/>
+      <c r="B68" s="102"/>
       <c r="C68" s="55" t="s">
         <v>131</v>
       </c>
       <c r="D68" s="27">
         <v>2</v>
       </c>
-      <c r="E68" s="106" t="s">
+      <c r="E68" s="88" t="s">
         <v>137</v>
       </c>
       <c r="F68" s="3"/>
@@ -4227,10 +4227,10 @@
       <c r="Z68" s="3"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="91"/>
+      <c r="B69" s="96"/>
       <c r="C69" s="55" t="s">
         <v>123</v>
       </c>
@@ -4295,10 +4295,10 @@
       <c r="Z70" s="3"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="90" t="s">
+      <c r="A71" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="91"/>
+      <c r="B71" s="96"/>
       <c r="C71" s="55" t="s">
         <v>38</v>
       </c>
@@ -4329,10 +4329,10 @@
       <c r="Z71" s="3"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="90" t="s">
+      <c r="A72" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="B72" s="91"/>
+      <c r="B72" s="96"/>
       <c r="C72" s="55" t="s">
         <v>48</v>
       </c>
@@ -4363,10 +4363,10 @@
       <c r="Z72" s="3"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="90" t="s">
+      <c r="A73" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="B73" s="91"/>
+      <c r="B73" s="96"/>
       <c r="C73" s="55" t="s">
         <v>44</v>
       </c>
@@ -4397,10 +4397,10 @@
       <c r="Z73" s="3"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="90" t="s">
+      <c r="A74" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="B74" s="91"/>
+      <c r="B74" s="96"/>
       <c r="C74" s="55" t="s">
         <v>46</v>
       </c>
@@ -4431,10 +4431,10 @@
       <c r="Z74" s="3"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="90" t="s">
+      <c r="A75" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="91"/>
+      <c r="B75" s="96"/>
       <c r="C75" s="55" t="s">
         <v>41</v>
       </c>
@@ -4465,10 +4465,10 @@
       <c r="Z75" s="3"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="90" t="s">
+      <c r="A76" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="B76" s="91"/>
+      <c r="B76" s="96"/>
       <c r="C76" s="55" t="s">
         <v>104</v>
       </c>
@@ -4499,10 +4499,10 @@
       <c r="Z76" s="3"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="B77" s="91"/>
+      <c r="B77" s="96"/>
       <c r="C77" s="55" t="s">
         <v>105</v>
       </c>
@@ -4595,10 +4595,10 @@
       <c r="B80" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="87" t="s">
+      <c r="C80" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="D80" s="87"/>
+      <c r="D80" s="92"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -4629,10 +4629,10 @@
       <c r="B81" s="54">
         <v>1</v>
       </c>
-      <c r="C81" s="88" t="s">
+      <c r="C81" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="D81" s="89"/>
+      <c r="D81" s="94"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -32517,17 +32517,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="94"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="99"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32722,17 +32722,17 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="94"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="99"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
@@ -32952,17 +32952,17 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="99" t="s">
+      <c r="A28" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="100"/>
-      <c r="C28" s="97"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="102"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="101" t="s">
+      <c r="A29" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="97"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="25" t="s">
         <v>34</v>
       </c>
@@ -32971,10 +32971,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="97"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="49" t="s">
         <v>27</v>
       </c>
@@ -32983,10 +32983,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="97"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="49" t="s">
         <v>38</v>
       </c>
@@ -32995,10 +32995,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="96" t="s">
+      <c r="A32" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="97"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="49" t="s">
         <v>48</v>
       </c>
@@ -33007,10 +33007,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="97"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="49" t="s">
         <v>44</v>
       </c>
@@ -33019,10 +33019,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="97"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="49" t="s">
         <v>46</v>
       </c>
@@ -33031,10 +33031,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="97"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="49" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Corrección perfil usuario, actualización de docs burndown chart, spring backlog
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66741E8D-68B0-44AD-BBF8-9B4D8439138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609A3F81-30E3-4B19-AF34-6A68E2C3A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="137">
   <si>
     <t>Universidad Nacional Mayor de San Marcos</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>alta</t>
-  </si>
-  <si>
-    <t>No iniciado</t>
   </si>
   <si>
     <t>Maquetar interfaces</t>
@@ -1351,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1686,7 +1683,7 @@
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="98"/>
       <c r="C11" s="98"/>
@@ -1716,19 +1713,19 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="85" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" s="87">
         <v>44559</v>
@@ -1740,10 +1737,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1764,19 +1761,19 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" s="85" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="87">
         <v>44559</v>
@@ -1788,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="86" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1812,16 +1809,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="85" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="86" t="s">
         <v>6</v>
@@ -1836,10 +1833,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="86" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1860,16 +1857,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="85" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="86" t="s">
         <v>6</v>
@@ -1884,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="86" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1908,19 +1905,19 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="69">
         <v>44560</v>
@@ -1932,7 +1929,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1954,16 +1951,16 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="68" t="s">
         <v>8</v>
@@ -1978,7 +1975,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2000,19 +1997,19 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="69">
         <v>44561</v>
@@ -2024,7 +2021,7 @@
         <v>4</v>
       </c>
       <c r="I18" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2046,16 +2043,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="68" t="s">
         <v>8</v>
@@ -2070,7 +2067,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2092,19 +2089,19 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" s="68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F20" s="69">
         <v>44565</v>
@@ -2116,7 +2113,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2138,19 +2135,19 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" s="73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F21" s="74">
         <v>44559</v>
@@ -2162,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="I21" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2184,16 +2181,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D22" s="73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="73" t="s">
         <v>6</v>
@@ -2208,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2230,19 +2227,19 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F23" s="74">
         <v>44560</v>
@@ -2254,7 +2251,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2276,16 +2273,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="73" t="s">
         <v>6</v>
@@ -2300,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="I24" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2322,19 +2319,19 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D25" s="73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="74">
         <v>44564</v>
@@ -2346,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2368,16 +2365,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>8</v>
@@ -2392,7 +2389,7 @@
         <v>4</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2414,19 +2411,19 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F27" s="21">
         <v>44566</v>
@@ -2438,7 +2435,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2460,19 +2457,19 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F28" s="21">
         <v>44567</v>
@@ -2484,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2506,16 +2503,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>8</v>
@@ -2530,7 +2527,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2552,19 +2549,19 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F30" s="21">
         <v>44571</v>
@@ -2576,7 +2573,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2598,19 +2595,19 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F31" s="59">
         <v>44566</v>
@@ -2622,7 +2619,7 @@
         <v>4</v>
       </c>
       <c r="I31" s="58" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2644,16 +2641,16 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="58" t="s">
         <v>6</v>
@@ -2668,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="58" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2690,19 +2687,19 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F33" s="59">
         <v>44567</v>
@@ -2714,7 +2711,7 @@
         <v>2</v>
       </c>
       <c r="I33" s="58" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2736,16 +2733,16 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>6</v>
@@ -2760,7 +2757,7 @@
         <v>4</v>
       </c>
       <c r="I34" s="58" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2782,19 +2779,19 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F35" s="59">
         <v>44571</v>
@@ -2806,7 +2803,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="58" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2828,19 +2825,19 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F36" s="16">
         <v>44572</v>
@@ -2852,7 +2849,7 @@
         <v>4</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2874,16 +2871,16 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>8</v>
@@ -2898,7 +2895,7 @@
         <v>4</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2920,19 +2917,19 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F38" s="16">
         <v>44573</v>
@@ -2944,7 +2941,7 @@
         <v>2</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2966,16 +2963,16 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>8</v>
@@ -2990,7 +2987,7 @@
         <v>4</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -3012,19 +3009,19 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F40" s="16">
         <v>44574</v>
@@ -3036,7 +3033,7 @@
         <v>4</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -3058,19 +3055,19 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="62" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F41" s="64">
         <v>44572</v>
@@ -3082,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="63" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -3104,16 +3101,16 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="62" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" s="63" t="s">
         <v>6</v>
@@ -3128,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="I42" s="63" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -3150,19 +3147,19 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="62" t="s">
         <v>20</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D43" s="63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E43" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F43" s="64">
         <v>44573</v>
@@ -3174,7 +3171,7 @@
         <v>2</v>
       </c>
       <c r="I43" s="63" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -3196,16 +3193,16 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="62" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E44" s="63" t="s">
         <v>6</v>
@@ -3220,7 +3217,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="63" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -3242,19 +3239,19 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="62" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F45" s="64">
         <v>44574</v>
@@ -3266,7 +3263,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="63" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -3288,19 +3285,19 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" s="68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E46" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F46" s="69">
         <v>44575</v>
@@ -3312,7 +3309,7 @@
         <v>4</v>
       </c>
       <c r="I46" s="68" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -3334,16 +3331,16 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D47" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>8</v>
@@ -3358,7 +3355,7 @@
         <v>2</v>
       </c>
       <c r="I47" s="68" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -3380,19 +3377,19 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E48" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F48" s="69">
         <v>44576</v>
@@ -3404,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="I48" s="68" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -3426,16 +3423,16 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E49" s="68" t="s">
         <v>8</v>
@@ -3450,7 +3447,7 @@
         <v>4</v>
       </c>
       <c r="I49" s="68" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3472,19 +3469,19 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C50" s="67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E50" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F50" s="69">
         <v>44578</v>
@@ -3496,7 +3493,7 @@
         <v>2</v>
       </c>
       <c r="I50" s="68" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -3518,19 +3515,19 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B51" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E51" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F51" s="74">
         <v>44575</v>
@@ -3542,7 +3539,7 @@
         <v>4</v>
       </c>
       <c r="I51" s="73" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -3564,16 +3561,16 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C52" s="72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" s="73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" s="73" t="s">
         <v>6</v>
@@ -3588,7 +3585,7 @@
         <v>4</v>
       </c>
       <c r="I52" s="73" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -3610,19 +3607,19 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C53" s="72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E53" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F53" s="74">
         <v>44576</v>
@@ -3634,7 +3631,7 @@
         <v>2</v>
       </c>
       <c r="I53" s="73" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -3656,16 +3653,16 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C54" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" s="73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E54" s="73" t="s">
         <v>6</v>
@@ -3680,7 +3677,7 @@
         <v>4</v>
       </c>
       <c r="I54" s="73" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -3702,19 +3699,19 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C55" s="72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E55" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F55" s="74">
         <v>44578</v>
@@ -3726,7 +3723,7 @@
         <v>4</v>
       </c>
       <c r="I55" s="73" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3748,16 +3745,16 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C56" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D56" s="78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E56" s="78" t="s">
         <v>8</v>
@@ -3772,7 +3769,7 @@
         <v>4</v>
       </c>
       <c r="I56" s="78" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -3794,16 +3791,16 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C57" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D57" s="78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" s="78" t="s">
         <v>6</v>
@@ -3818,7 +3815,7 @@
         <v>4</v>
       </c>
       <c r="I57" s="78" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3840,16 +3837,16 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C58" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D58" s="78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E58" s="78" t="s">
         <v>6</v>
@@ -3864,7 +3861,7 @@
         <v>2</v>
       </c>
       <c r="I58" s="78" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3886,16 +3883,16 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C59" s="77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D59" s="78" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E59" s="78" t="s">
         <v>8</v>
@@ -3910,7 +3907,7 @@
         <v>4</v>
       </c>
       <c r="I59" s="78" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3932,16 +3929,16 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B60" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C60" s="77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D60" s="78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E60" s="78" t="s">
         <v>6</v>
@@ -3956,7 +3953,7 @@
         <v>4</v>
       </c>
       <c r="I60" s="78" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3978,7 +3975,7 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -4092,7 +4089,7 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="89" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B65" s="90"/>
       <c r="C65" s="90"/>
@@ -4122,14 +4119,14 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="100" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B66" s="91"/>
       <c r="C66" s="51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D66" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -4156,17 +4153,17 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B67" s="102"/>
       <c r="C67" s="55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D67" s="27">
         <v>2</v>
       </c>
       <c r="E67" s="88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -4192,17 +4189,17 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68" s="27">
         <v>2</v>
       </c>
       <c r="E68" s="88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -4228,11 +4225,11 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B69" s="96"/>
       <c r="C69" s="55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D69" s="27">
         <v>28</v>
@@ -4262,11 +4259,11 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="82"/>
       <c r="C70" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D70" s="27">
         <v>14</v>
@@ -4296,11 +4293,11 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B71" s="96"/>
       <c r="C71" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" s="27">
         <v>18</v>
@@ -4330,11 +4327,11 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="95" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" s="96"/>
       <c r="C72" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D72" s="27">
         <v>18</v>
@@ -4364,11 +4361,11 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="95" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B73" s="96"/>
       <c r="C73" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D73" s="27">
         <v>18</v>
@@ -4398,11 +4395,11 @@
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B74" s="96"/>
       <c r="C74" s="55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D74" s="27">
         <v>10</v>
@@ -4432,11 +4429,11 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B75" s="96"/>
       <c r="C75" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D75" s="27">
         <v>14</v>
@@ -4466,11 +4463,11 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="95" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B76" s="96"/>
       <c r="C76" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D76" s="27">
         <v>18</v>
@@ -4500,11 +4497,11 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B77" s="96"/>
       <c r="C77" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D77" s="27">
         <v>18</v>
@@ -4590,13 +4587,13 @@
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="52" t="s">
+      <c r="C80" s="92" t="s">
         <v>87</v>
-      </c>
-      <c r="C80" s="92" t="s">
-        <v>88</v>
       </c>
       <c r="D80" s="92"/>
       <c r="E80" s="3"/>
@@ -4630,7 +4627,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D81" s="94"/>
       <c r="E81" s="3"/>
@@ -31292,43 +31289,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>38</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>19</v>
@@ -31336,26 +31333,26 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32394,7 +32391,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -32407,14 +32404,14 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -32437,7 +32434,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -32463,11 +32460,11 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -32532,19 +32529,19 @@
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="35" t="s">
         <v>55</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>56</v>
       </c>
       <c r="F12" s="36">
         <v>44368</v>
@@ -32556,24 +32553,24 @@
         <v>6</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="41" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>59</v>
       </c>
       <c r="F13" s="42">
         <v>44375</v>
@@ -32585,7 +32582,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -32607,19 +32604,19 @@
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="33" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="36">
         <v>44377</v>
@@ -32631,24 +32628,24 @@
         <v>10</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>61</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>62</v>
       </c>
       <c r="F15" s="44">
         <v>44370</v>
@@ -32660,24 +32657,24 @@
         <v>9</v>
       </c>
       <c r="I15" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="33" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>64</v>
-      </c>
       <c r="E16" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="36">
         <v>44372</v>
@@ -32689,24 +32686,24 @@
         <v>10</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>65</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>66</v>
       </c>
       <c r="F17" s="36">
         <v>44383</v>
@@ -32718,12 +32715,12 @@
         <v>6</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="98"/>
       <c r="C18" s="98"/>
@@ -32736,19 +32733,19 @@
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="47">
         <v>44397</v>
@@ -32760,24 +32757,24 @@
         <v>10</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="D20" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="48" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>71</v>
       </c>
       <c r="F20" s="44">
         <v>44407</v>
@@ -32789,24 +32786,24 @@
         <v>6</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="44">
         <v>44410</v>
@@ -32818,24 +32815,24 @@
         <v>10</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="35" t="s">
         <v>73</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>74</v>
       </c>
       <c r="F22" s="44">
         <v>44415</v>
@@ -32847,24 +32844,24 @@
         <v>6</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="44">
         <v>44418</v>
@@ -32876,24 +32873,24 @@
         <v>10</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="D24" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="35" t="s">
         <v>77</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>78</v>
       </c>
       <c r="F24" s="44">
         <v>44424</v>
@@ -32905,24 +32902,24 @@
         <v>6</v>
       </c>
       <c r="I24" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>80</v>
       </c>
       <c r="F25" s="44">
         <v>44427</v>
@@ -32934,12 +32931,12 @@
         <v>10</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -32953,30 +32950,30 @@
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="105"/>
       <c r="C28" s="102"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="106" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="102"/>
       <c r="C29" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="26" t="s">
         <v>34</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="101" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="102"/>
       <c r="C30" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="50">
         <v>24</v>
@@ -32984,11 +32981,11 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="101" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="102"/>
       <c r="C31" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="26">
         <v>24</v>
@@ -32996,11 +32993,11 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="102"/>
       <c r="C32" s="49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="26">
         <v>20</v>
@@ -33008,11 +33005,11 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="101" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="102"/>
       <c r="C33" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="50">
         <v>20</v>
@@ -33020,11 +33017,11 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="102"/>
       <c r="C34" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="50">
         <v>20</v>
@@ -33032,11 +33029,11 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="101" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="102"/>
       <c r="C35" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="50">
         <v>20</v>

</xml_diff>

<commit_message>
Actualización de documentos Sprint 3
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 3/Sprint Backlog - S3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609A3F81-30E3-4B19-AF34-6A68E2C3A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB553565-4133-4F58-9DB3-0B47D436CF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="141">
   <si>
     <t>Universidad Nacional Mayor de San Marcos</t>
   </si>
@@ -423,9 +423,6 @@
     <t>Tarea 4 (T02-T4)</t>
   </si>
   <si>
-    <t>Iniciado</t>
-  </si>
-  <si>
     <t>Tarea 5 (T02-T5)</t>
   </si>
   <si>
@@ -448,6 +445,21 @@
   </si>
   <si>
     <t>HU pendiente del Sprint 3</t>
+  </si>
+  <si>
+    <t>Tarea 1 (A07-T1)</t>
+  </si>
+  <si>
+    <t>Tarea 2 (A07-T2)</t>
+  </si>
+  <si>
+    <t>Tarea 3 (A07-T3)</t>
+  </si>
+  <si>
+    <t>Tarea 4 (A07-T4)</t>
+  </si>
+  <si>
+    <t>Tarea 5 (A07-T5)</t>
   </si>
 </sst>
 </file>
@@ -1348,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:B76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1725,13 +1737,13 @@
         <v>24</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" s="87">
+        <v>44558</v>
+      </c>
+      <c r="G12" s="87">
         <v>44559</v>
-      </c>
-      <c r="G12" s="87">
-        <v>44560</v>
       </c>
       <c r="H12" s="85">
         <v>1</v>
@@ -1740,7 +1752,7 @@
         <v>56</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1767,19 +1779,19 @@
         <v>20</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="86" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F13" s="87">
+        <v>44558</v>
+      </c>
+      <c r="G13" s="87">
         <v>44559</v>
-      </c>
-      <c r="G13" s="87">
-        <v>44560</v>
       </c>
       <c r="H13" s="85">
         <v>1</v>
@@ -1788,7 +1800,7 @@
         <v>56</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1809,7 +1821,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="85" t="s">
         <v>20</v>
@@ -1836,7 +1848,7 @@
         <v>56</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1857,13 +1869,13 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="85" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="86" t="s">
         <v>25</v>
@@ -1884,7 +1896,7 @@
         <v>56</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -2527,7 +2539,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2573,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2757,7 +2769,7 @@
         <v>4</v>
       </c>
       <c r="I34" s="58" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2803,7 +2815,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="58" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2987,7 +2999,7 @@
         <v>4</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -3033,7 +3045,7 @@
         <v>4</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -3217,7 +3229,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="63" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -3263,7 +3275,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="63" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -3447,7 +3459,7 @@
         <v>4</v>
       </c>
       <c r="I49" s="68" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3493,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="I50" s="68" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -3677,7 +3689,7 @@
         <v>4</v>
       </c>
       <c r="I54" s="73" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -3723,7 +3735,7 @@
         <v>4</v>
       </c>
       <c r="I55" s="73" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3745,13 +3757,13 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B56" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C56" s="77" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="D56" s="78" t="s">
         <v>21</v>
@@ -3791,13 +3803,13 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B57" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C57" s="77" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="D57" s="78" t="s">
         <v>22</v>
@@ -3837,13 +3849,13 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B58" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C58" s="77" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="D58" s="78" t="s">
         <v>23</v>
@@ -3883,13 +3895,13 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B59" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C59" s="77" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="D59" s="78" t="s">
         <v>24</v>
@@ -3907,7 +3919,7 @@
         <v>4</v>
       </c>
       <c r="I59" s="78" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3929,13 +3941,13 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B60" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C60" s="77" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D60" s="78" t="s">
         <v>25</v>
@@ -3953,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="I60" s="78" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -4153,7 +4165,7 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="101" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="102"/>
       <c r="C67" s="55" t="s">
@@ -4163,7 +4175,7 @@
         <v>2</v>
       </c>
       <c r="E67" s="88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -4189,17 +4201,17 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D68" s="27">
         <v>2</v>
       </c>
       <c r="E68" s="88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>

</xml_diff>